<commit_message>
all data cleaned and grpahs plotted
</commit_message>
<xml_diff>
--- a/Testing/IMU data/joltAccel.xlsx
+++ b/Testing/IMU data/joltAccel.xlsx
@@ -8,21 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tris/Documents/2022UCT/2nd sem/3097/SHARC_buoy_data_transmission/Testing/IMU data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11466B4F-3502-8045-BBCF-CED75459662F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{402971B5-B25A-564A-8F1B-91509035360C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{E481E891-027F-FB4E-AA14-C9B15BFD56E2}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{E481E891-027F-FB4E-AA14-C9B15BFD56E2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$A$2:$A$60</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$B$2:$B$60</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Sheet1!$C$2:$C$60</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Sheet1!$A$2:$A$60</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">Sheet1!$B$2:$B$60</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">Sheet1!$C$2:$C$60</definedName>
-  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -839,6 +831,66 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Time</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t> (100 ms)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -904,6 +956,66 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Acceleration</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t> (m/s)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1576,13 +1688,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>7054</xdr:colOff>
+      <xdr:colOff>7053</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>161380</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>599722</xdr:colOff>
+      <xdr:colOff>770466</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>70555</xdr:rowOff>
     </xdr:to>
@@ -1911,8 +2023,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8304FF5-9DFE-0745-991E-B77A23D4D323}">
   <dimension ref="A1:C60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="230" workbookViewId="0">
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>